<commit_message>
Update: updated for v1.9
</commit_message>
<xml_diff>
--- a/uploads/xlsx/Timetable SE Department (Fall-25) Version-1.9.xlsx
+++ b/uploads/xlsx/Timetable SE Department (Fall-25) Version-1.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zPythonStuff\Superior Academic Tool\uploads\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61B50A2-E55F-4549-B6BF-508979DB5132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C0B4DC-7E66-4589-BB58-1C4861EB59B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="577" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="352">
   <si>
     <t>Department fo Software Engineering {Monday to Friday Timetable Fall-25}</t>
   </si>
@@ -2529,16 +2529,6 @@
 Mr. Muhammad Usman Khan  </t>
   </si>
   <si>
-    <t>Discrete Structures
-BSSE-1D
-Dr. Hafiz Muhammad Tayyab Khushi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discrete Structures
-BSSE-1D
-Dr. Hafiz Muhammad Tayyab Khushi  </t>
-  </si>
-  <si>
     <t>Analysis of Algorithms 
 BSAI-5C/BSDS-5A
 Mr. Nagesh Kumar</t>
@@ -2591,6 +2581,11 @@
       </rPr>
       <t xml:space="preserve">Dr. Rehman Fazal </t>
     </r>
+  </si>
+  <si>
+    <t>Discrete Structures
+BSSE-1D
+Dr. Tehreem Masood</t>
   </si>
   <si>
     <r>
@@ -5231,12 +5226,576 @@
     <xf numFmtId="0" fontId="10" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="130" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="132" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="131" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="116" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="118" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="127" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="122" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5261,21 +5820,12 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5288,577 +5838,22 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="122" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="7" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="7" borderId="130" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="127" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="116" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="118" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="131" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="124" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="132" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6123,8 +6118,8 @@
   <dimension ref="A1:AB1004"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27:I27"/>
+      <pane ySplit="5" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6149,10 +6144,10 @@
       <c r="D1" s="31"/>
       <c r="E1" s="31"/>
       <c r="F1" s="31"/>
-      <c r="G1" s="321"/>
-      <c r="H1" s="322"/>
-      <c r="I1" s="322"/>
-      <c r="J1" s="323"/>
+      <c r="G1" s="339"/>
+      <c r="H1" s="340"/>
+      <c r="I1" s="340"/>
+      <c r="J1" s="341"/>
       <c r="K1" s="128"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -6173,20 +6168,20 @@
       <c r="AB1" s="3"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="324" t="s">
+      <c r="A2" s="343" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="325"/>
-      <c r="C2" s="325"/>
-      <c r="D2" s="325"/>
-      <c r="E2" s="325"/>
+      <c r="B2" s="344"/>
+      <c r="C2" s="344"/>
+      <c r="D2" s="344"/>
+      <c r="E2" s="344"/>
       <c r="F2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="248"/>
-      <c r="H2" s="248"/>
-      <c r="I2" s="248"/>
-      <c r="J2" s="248"/>
+      <c r="G2" s="342"/>
+      <c r="H2" s="342"/>
+      <c r="I2" s="342"/>
+      <c r="J2" s="342"/>
       <c r="K2" s="129"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -6207,18 +6202,18 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="326"/>
-      <c r="B3" s="327"/>
-      <c r="C3" s="327"/>
-      <c r="D3" s="327"/>
-      <c r="E3" s="244"/>
+      <c r="A3" s="220"/>
+      <c r="B3" s="305"/>
+      <c r="C3" s="305"/>
+      <c r="D3" s="305"/>
+      <c r="E3" s="231"/>
       <c r="F3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="328"/>
-      <c r="H3" s="239"/>
-      <c r="I3" s="239"/>
-      <c r="J3" s="239"/>
+      <c r="G3" s="345"/>
+      <c r="H3" s="225"/>
+      <c r="I3" s="225"/>
+      <c r="J3" s="225"/>
       <c r="K3" s="130"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -6239,18 +6234,18 @@
       <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="326"/>
-      <c r="B4" s="244"/>
-      <c r="C4" s="244"/>
-      <c r="D4" s="244"/>
-      <c r="E4" s="244"/>
+      <c r="A4" s="220"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
       <c r="F4" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="329"/>
-      <c r="H4" s="330"/>
-      <c r="I4" s="330"/>
-      <c r="J4" s="330"/>
+      <c r="G4" s="346"/>
+      <c r="H4" s="294"/>
+      <c r="I4" s="294"/>
+      <c r="J4" s="294"/>
       <c r="K4" s="131"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -6272,10 +6267,10 @@
     </row>
     <row r="5" spans="1:28" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="82"/>
-      <c r="B5" s="331" t="s">
+      <c r="B5" s="347" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="332"/>
+      <c r="C5" s="348"/>
       <c r="D5" s="83" t="s">
         <v>3</v>
       </c>
@@ -6351,7 +6346,7 @@
       <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="222"/>
+      <c r="A7" s="410"/>
       <c r="B7" s="33" t="s">
         <v>221</v>
       </c>
@@ -6364,14 +6359,14 @@
       <c r="E7" s="152" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="390" t="s">
+      <c r="F7" s="255" t="s">
         <v>219</v>
       </c>
-      <c r="G7" s="391"/>
-      <c r="H7" s="391"/>
-      <c r="I7" s="391"/>
-      <c r="J7" s="391"/>
-      <c r="K7" s="392"/>
+      <c r="G7" s="256"/>
+      <c r="H7" s="256"/>
+      <c r="I7" s="256"/>
+      <c r="J7" s="256"/>
+      <c r="K7" s="257"/>
       <c r="L7" s="109"/>
       <c r="M7" s="109"/>
       <c r="N7" s="109"/>
@@ -6391,11 +6386,11 @@
       <c r="AB7" s="110"/>
     </row>
     <row r="8" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="223"/>
+      <c r="A8" s="411"/>
       <c r="B8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="337" t="s">
+      <c r="C8" s="353" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="44" t="s">
@@ -6416,10 +6411,10 @@
       <c r="I8" s="120" t="s">
         <v>114</v>
       </c>
-      <c r="J8" s="227" t="s">
+      <c r="J8" s="356" t="s">
         <v>198</v>
       </c>
-      <c r="K8" s="228"/>
+      <c r="K8" s="415"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -6439,26 +6434,26 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="223"/>
+      <c r="A9" s="411"/>
       <c r="B9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="334"/>
-      <c r="D9" s="251" t="s">
+      <c r="C9" s="350"/>
+      <c r="D9" s="424" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="252"/>
-      <c r="F9" s="233" t="s">
+      <c r="E9" s="335"/>
+      <c r="F9" s="418" t="s">
         <v>295</v>
       </c>
-      <c r="G9" s="257"/>
+      <c r="G9" s="426"/>
       <c r="H9" s="157" t="s">
         <v>100</v>
       </c>
-      <c r="I9" s="407" t="s">
+      <c r="I9" s="280" t="s">
         <v>129</v>
       </c>
-      <c r="J9" s="239"/>
+      <c r="J9" s="225"/>
       <c r="K9" s="155" t="s">
         <v>199</v>
       </c>
@@ -6481,11 +6476,11 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="223"/>
+      <c r="A10" s="411"/>
       <c r="B10" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="334"/>
+      <c r="C10" s="350"/>
       <c r="D10" s="214"/>
       <c r="E10" s="216" t="s">
         <v>329</v>
@@ -6493,10 +6488,10 @@
       <c r="F10" s="216" t="s">
         <v>234</v>
       </c>
-      <c r="G10" s="219" t="s">
+      <c r="G10" s="407" t="s">
         <v>280</v>
       </c>
-      <c r="H10" s="219"/>
+      <c r="H10" s="407"/>
       <c r="I10" s="198" t="s">
         <v>53</v>
       </c>
@@ -6525,11 +6520,11 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="223"/>
+      <c r="A11" s="411"/>
       <c r="B11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="333" t="s">
+      <c r="C11" s="349" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="198" t="s">
@@ -6544,14 +6539,14 @@
       <c r="G11" s="180" t="s">
         <v>241</v>
       </c>
-      <c r="H11" s="236" t="s">
+      <c r="H11" s="287" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="237"/>
-      <c r="J11" s="319" t="s">
+      <c r="I11" s="238"/>
+      <c r="J11" s="264" t="s">
         <v>97</v>
       </c>
-      <c r="K11" s="287"/>
+      <c r="K11" s="337"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -6571,29 +6566,29 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="223"/>
+      <c r="A12" s="411"/>
       <c r="B12" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="334"/>
-      <c r="D12" s="346" t="s">
+      <c r="C12" s="350"/>
+      <c r="D12" s="359" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="255"/>
+      <c r="E12" s="313"/>
       <c r="F12" s="71" t="s">
         <v>47</v>
       </c>
       <c r="G12" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="253" t="s">
+      <c r="H12" s="221" t="s">
         <v>273</v>
       </c>
-      <c r="I12" s="246"/>
-      <c r="J12" s="238" t="s">
+      <c r="I12" s="227"/>
+      <c r="J12" s="224" t="s">
         <v>152</v>
       </c>
-      <c r="K12" s="287"/>
+      <c r="K12" s="337"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -6613,29 +6608,29 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="223"/>
+      <c r="A13" s="411"/>
       <c r="B13" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="334"/>
-      <c r="D13" s="254" t="s">
+      <c r="C13" s="350"/>
+      <c r="D13" s="425" t="s">
         <v>226</v>
       </c>
-      <c r="E13" s="255"/>
+      <c r="E13" s="313"/>
       <c r="F13" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="229" t="s">
+      <c r="G13" s="336" t="s">
         <v>334</v>
       </c>
-      <c r="H13" s="252"/>
+      <c r="H13" s="335"/>
       <c r="I13" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="229" t="s">
+      <c r="J13" s="336" t="s">
         <v>306</v>
       </c>
-      <c r="K13" s="230"/>
+      <c r="K13" s="416"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -6655,11 +6650,11 @@
       <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="223"/>
+      <c r="A14" s="411"/>
       <c r="B14" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="334"/>
+      <c r="C14" s="350"/>
       <c r="D14" s="38" t="s">
         <v>121</v>
       </c>
@@ -6669,10 +6664,10 @@
       <c r="F14" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="G14" s="256" t="s">
+      <c r="G14" s="368" t="s">
         <v>264</v>
       </c>
-      <c r="H14" s="256"/>
+      <c r="H14" s="368"/>
       <c r="I14" s="38" t="s">
         <v>180</v>
       </c>
@@ -6699,29 +6694,29 @@
       <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="223"/>
+      <c r="A15" s="411"/>
       <c r="B15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="335"/>
+      <c r="C15" s="351"/>
       <c r="D15" s="215" t="s">
         <v>330</v>
       </c>
-      <c r="E15" s="220" t="s">
+      <c r="E15" s="408" t="s">
         <v>324</v>
       </c>
-      <c r="F15" s="221"/>
+      <c r="F15" s="409"/>
       <c r="G15" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="H15" s="253" t="s">
+      <c r="H15" s="221" t="s">
         <v>305</v>
       </c>
-      <c r="I15" s="246"/>
-      <c r="J15" s="286" t="s">
+      <c r="I15" s="227"/>
+      <c r="J15" s="296" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="287"/>
+      <c r="K15" s="337"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -6741,25 +6736,25 @@
       <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="223"/>
+      <c r="A16" s="411"/>
       <c r="B16" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="334"/>
-      <c r="D16" s="279" t="s">
+      <c r="C16" s="350"/>
+      <c r="D16" s="401" t="s">
         <v>219</v>
       </c>
-      <c r="E16" s="280"/>
-      <c r="F16" s="347" t="s">
+      <c r="E16" s="402"/>
+      <c r="F16" s="360" t="s">
         <v>130</v>
       </c>
-      <c r="G16" s="330"/>
-      <c r="H16" s="258" t="s">
+      <c r="G16" s="294"/>
+      <c r="H16" s="386" t="s">
         <v>210</v>
       </c>
-      <c r="I16" s="259"/>
-      <c r="J16" s="259"/>
-      <c r="K16" s="260"/>
+      <c r="I16" s="387"/>
+      <c r="J16" s="387"/>
+      <c r="K16" s="388"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -6779,27 +6774,27 @@
       <c r="AB16" s="3"/>
     </row>
     <row r="17" spans="1:28" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="223"/>
+      <c r="A17" s="411"/>
       <c r="B17" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="334"/>
-      <c r="D17" s="238" t="s">
+      <c r="C17" s="350"/>
+      <c r="D17" s="224" t="s">
         <v>281</v>
       </c>
-      <c r="E17" s="239"/>
-      <c r="F17" s="253" t="s">
+      <c r="E17" s="225"/>
+      <c r="F17" s="221" t="s">
         <v>151</v>
       </c>
-      <c r="G17" s="274"/>
-      <c r="H17" s="253" t="s">
+      <c r="G17" s="317"/>
+      <c r="H17" s="221" t="s">
         <v>291</v>
       </c>
-      <c r="I17" s="246"/>
-      <c r="J17" s="338" t="s">
+      <c r="I17" s="227"/>
+      <c r="J17" s="354" t="s">
         <v>46</v>
       </c>
-      <c r="K17" s="339"/>
+      <c r="K17" s="355"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -6819,23 +6814,23 @@
       <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="1:28" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="223"/>
+      <c r="A18" s="411"/>
       <c r="B18" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="334"/>
-      <c r="D18" s="348" t="s">
+      <c r="C18" s="350"/>
+      <c r="D18" s="321" t="s">
         <v>278</v>
       </c>
-      <c r="E18" s="349"/>
-      <c r="F18" s="253" t="s">
+      <c r="E18" s="290"/>
+      <c r="F18" s="221" t="s">
         <v>337</v>
       </c>
-      <c r="G18" s="246"/>
-      <c r="H18" s="253" t="s">
+      <c r="G18" s="227"/>
+      <c r="H18" s="221" t="s">
         <v>338</v>
       </c>
-      <c r="I18" s="246"/>
+      <c r="I18" s="227"/>
       <c r="J18" s="39" t="s">
         <v>179</v>
       </c>
@@ -6861,23 +6856,23 @@
       <c r="AB18" s="3"/>
     </row>
     <row r="19" spans="1:28" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="223"/>
+      <c r="A19" s="411"/>
       <c r="B19" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="334"/>
-      <c r="D19" s="238" t="s">
+      <c r="C19" s="350"/>
+      <c r="D19" s="224" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="340"/>
-      <c r="F19" s="227" t="s">
+      <c r="E19" s="244"/>
+      <c r="F19" s="356" t="s">
         <v>150</v>
       </c>
-      <c r="G19" s="248"/>
-      <c r="H19" s="253" t="s">
+      <c r="G19" s="342"/>
+      <c r="H19" s="221" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="246"/>
+      <c r="I19" s="227"/>
       <c r="J19" s="10"/>
       <c r="K19" s="97"/>
       <c r="L19" s="2"/>
@@ -6899,23 +6894,23 @@
       <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="224"/>
+      <c r="A20" s="412"/>
       <c r="B20" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="336"/>
-      <c r="D20" s="341" t="s">
+      <c r="C20" s="352"/>
+      <c r="D20" s="357" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="342"/>
-      <c r="F20" s="343" t="s">
+      <c r="E20" s="307"/>
+      <c r="F20" s="306" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="342"/>
-      <c r="H20" s="344" t="s">
+      <c r="G20" s="307"/>
+      <c r="H20" s="358" t="s">
         <v>108</v>
       </c>
-      <c r="I20" s="345"/>
+      <c r="I20" s="279"/>
       <c r="J20" s="73" t="s">
         <v>128</v>
       </c>
@@ -6940,10 +6935,10 @@
     </row>
     <row r="21" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="46"/>
-      <c r="B21" s="409" t="s">
+      <c r="B21" s="217" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="410"/>
+      <c r="C21" s="218"/>
       <c r="D21" s="47"/>
       <c r="E21" s="48"/>
       <c r="F21" s="48"/>
@@ -6971,7 +6966,7 @@
       <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="265" t="s">
+      <c r="A22" s="391" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="122" t="s">
@@ -7021,7 +7016,7 @@
       <c r="AB22" s="3"/>
     </row>
     <row r="23" spans="1:28" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="266"/>
+      <c r="A23" s="392"/>
       <c r="B23" s="64" t="s">
         <v>220</v>
       </c>
@@ -7032,14 +7027,14 @@
       <c r="E23" s="39" t="s">
         <v>245</v>
       </c>
-      <c r="F23" s="390" t="s">
+      <c r="F23" s="255" t="s">
         <v>219</v>
       </c>
-      <c r="G23" s="391"/>
-      <c r="H23" s="391"/>
-      <c r="I23" s="391"/>
-      <c r="J23" s="391"/>
-      <c r="K23" s="392"/>
+      <c r="G23" s="256"/>
+      <c r="H23" s="256"/>
+      <c r="I23" s="256"/>
+      <c r="J23" s="256"/>
+      <c r="K23" s="257"/>
       <c r="L23" s="109"/>
       <c r="M23" s="109"/>
       <c r="N23" s="109"/>
@@ -7059,31 +7054,31 @@
       <c r="AB23" s="110"/>
     </row>
     <row r="24" spans="1:28" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="267"/>
+      <c r="A24" s="284"/>
       <c r="B24" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="411" t="s">
+      <c r="C24" s="219" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="243" t="s">
+      <c r="D24" s="241" t="s">
         <v>228</v>
       </c>
-      <c r="E24" s="244"/>
+      <c r="E24" s="231"/>
       <c r="F24" s="44" t="s">
         <v>251</v>
       </c>
       <c r="G24" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="H24" s="245" t="s">
+      <c r="H24" s="422" t="s">
         <v>117</v>
       </c>
-      <c r="I24" s="246"/>
-      <c r="J24" s="261" t="s">
+      <c r="I24" s="227"/>
+      <c r="J24" s="269" t="s">
         <v>212</v>
       </c>
-      <c r="K24" s="262"/>
+      <c r="K24" s="270"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -7103,29 +7098,29 @@
       <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="1:28" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="267"/>
+      <c r="A25" s="284"/>
       <c r="B25" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="326"/>
-      <c r="D25" s="240" t="s">
+      <c r="C25" s="220"/>
+      <c r="D25" s="397" t="s">
         <v>229</v>
       </c>
-      <c r="E25" s="275"/>
+      <c r="E25" s="398"/>
       <c r="F25" s="153" t="s">
         <v>270</v>
       </c>
       <c r="G25" s="154" t="s">
         <v>230</v>
       </c>
-      <c r="H25" s="247" t="s">
+      <c r="H25" s="399" t="s">
         <v>296</v>
       </c>
-      <c r="I25" s="237"/>
-      <c r="J25" s="240" t="s">
+      <c r="I25" s="238"/>
+      <c r="J25" s="397" t="s">
         <v>144</v>
       </c>
-      <c r="K25" s="241"/>
+      <c r="K25" s="421"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -7145,29 +7140,29 @@
       <c r="AB25" s="3"/>
     </row>
     <row r="26" spans="1:28" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="267"/>
+      <c r="A26" s="284"/>
       <c r="B26" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="326"/>
-      <c r="D26" s="315" t="s">
+      <c r="C26" s="220"/>
+      <c r="D26" s="384" t="s">
         <v>310</v>
       </c>
-      <c r="E26" s="316"/>
+      <c r="E26" s="385"/>
       <c r="F26" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="227" t="s">
+      <c r="G26" s="356" t="s">
         <v>165</v>
       </c>
-      <c r="H26" s="278"/>
+      <c r="H26" s="400"/>
       <c r="I26" s="157" t="s">
         <v>203</v>
       </c>
-      <c r="J26" s="291" t="s">
+      <c r="J26" s="365" t="s">
         <v>124</v>
       </c>
-      <c r="K26" s="292"/>
+      <c r="K26" s="366"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -7187,25 +7182,25 @@
       <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="1:28" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="267"/>
+      <c r="A27" s="284"/>
       <c r="B27" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="269" t="s">
+      <c r="C27" s="286" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="249" t="s">
+      <c r="D27" s="282" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="250"/>
-      <c r="F27" s="225" t="s">
+      <c r="E27" s="423"/>
+      <c r="F27" s="413" t="s">
         <v>262</v>
       </c>
-      <c r="G27" s="226"/>
-      <c r="H27" s="253" t="s">
+      <c r="G27" s="414"/>
+      <c r="H27" s="221" t="s">
         <v>214</v>
       </c>
-      <c r="I27" s="246"/>
+      <c r="I27" s="227"/>
       <c r="J27" s="44" t="s">
         <v>155</v>
       </c>
@@ -7231,23 +7226,23 @@
       <c r="AB27" s="3"/>
     </row>
     <row r="28" spans="1:28" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="267"/>
+      <c r="A28" s="284"/>
       <c r="B28" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="267"/>
-      <c r="D28" s="282" t="s">
+      <c r="C28" s="284"/>
+      <c r="D28" s="404" t="s">
         <v>263</v>
       </c>
-      <c r="E28" s="283"/>
-      <c r="F28" s="253" t="s">
+      <c r="E28" s="405"/>
+      <c r="F28" s="221" t="s">
         <v>316</v>
       </c>
-      <c r="G28" s="253"/>
-      <c r="H28" s="247" t="s">
+      <c r="G28" s="221"/>
+      <c r="H28" s="399" t="s">
         <v>98</v>
       </c>
-      <c r="I28" s="237"/>
+      <c r="I28" s="238"/>
       <c r="J28" s="34" t="s">
         <v>127</v>
       </c>
@@ -7271,21 +7266,21 @@
       <c r="AB28" s="3"/>
     </row>
     <row r="29" spans="1:28" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="267"/>
+      <c r="A29" s="284"/>
       <c r="B29" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="267"/>
+      <c r="C29" s="284"/>
       <c r="D29" s="195" t="s">
         <v>330</v>
       </c>
       <c r="E29" s="147" t="s">
         <v>236</v>
       </c>
-      <c r="F29" s="308" t="s">
+      <c r="F29" s="379" t="s">
         <v>275</v>
       </c>
-      <c r="G29" s="246"/>
+      <c r="G29" s="227"/>
       <c r="H29" s="158" t="s">
         <v>253</v>
       </c>
@@ -7315,21 +7310,21 @@
       <c r="AB29" s="3"/>
     </row>
     <row r="30" spans="1:28" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="267"/>
+      <c r="A30" s="284"/>
       <c r="B30" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="267"/>
+      <c r="C30" s="284"/>
       <c r="D30" s="38" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F30" s="309" t="s">
-        <v>351</v>
-      </c>
-      <c r="G30" s="310"/>
+      <c r="F30" s="380" t="s">
+        <v>349</v>
+      </c>
+      <c r="G30" s="381"/>
       <c r="H30" s="39" t="s">
         <v>321</v>
       </c>
@@ -7359,26 +7354,26 @@
       <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="1:28" ht="63" x14ac:dyDescent="0.25">
-      <c r="A31" s="267"/>
+      <c r="A31" s="284"/>
       <c r="B31" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="267"/>
-      <c r="D31" s="276" t="s">
+      <c r="C31" s="284"/>
+      <c r="D31" s="271" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="277"/>
-      <c r="F31" s="318" t="s">
+      <c r="E31" s="272"/>
+      <c r="F31" s="334" t="s">
         <v>125</v>
       </c>
-      <c r="G31" s="252"/>
+      <c r="G31" s="335"/>
       <c r="H31" s="132" t="s">
         <v>114</v>
       </c>
-      <c r="I31" s="229" t="s">
+      <c r="I31" s="336" t="s">
         <v>163</v>
       </c>
-      <c r="J31" s="239"/>
+      <c r="J31" s="225"/>
       <c r="K31" s="97"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -7399,27 +7394,27 @@
       <c r="AB31" s="3"/>
     </row>
     <row r="32" spans="1:28" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="267"/>
+      <c r="A32" s="284"/>
       <c r="B32" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="267"/>
-      <c r="D32" s="272" t="s">
-        <v>352</v>
-      </c>
-      <c r="E32" s="273"/>
-      <c r="F32" s="281" t="s">
+      <c r="C32" s="284"/>
+      <c r="D32" s="395" t="s">
+        <v>351</v>
+      </c>
+      <c r="E32" s="396"/>
+      <c r="F32" s="403" t="s">
         <v>219</v>
       </c>
-      <c r="G32" s="281"/>
-      <c r="H32" s="311" t="s">
+      <c r="G32" s="403"/>
+      <c r="H32" s="382" t="s">
         <v>219</v>
       </c>
-      <c r="I32" s="312"/>
-      <c r="J32" s="284" t="s">
+      <c r="I32" s="383"/>
+      <c r="J32" s="363" t="s">
         <v>166</v>
       </c>
-      <c r="K32" s="290"/>
+      <c r="K32" s="364"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -7439,29 +7434,29 @@
       <c r="AB32" s="3"/>
     </row>
     <row r="33" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="267"/>
+      <c r="A33" s="284"/>
       <c r="B33" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="267"/>
+      <c r="C33" s="284"/>
       <c r="D33" s="160" t="s">
         <v>237</v>
       </c>
       <c r="E33" s="193" t="s">
         <v>311</v>
       </c>
-      <c r="F33" s="317" t="s">
+      <c r="F33" s="267" t="s">
         <v>189</v>
       </c>
-      <c r="G33" s="246"/>
-      <c r="H33" s="231" t="s">
+      <c r="G33" s="227"/>
+      <c r="H33" s="316" t="s">
         <v>188</v>
       </c>
-      <c r="I33" s="232"/>
-      <c r="J33" s="233" t="s">
+      <c r="I33" s="417"/>
+      <c r="J33" s="418" t="s">
         <v>202</v>
       </c>
-      <c r="K33" s="234"/>
+      <c r="K33" s="419"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -7481,27 +7476,27 @@
       <c r="AB33" s="3"/>
     </row>
     <row r="34" spans="1:28" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="267"/>
+      <c r="A34" s="284"/>
       <c r="B34" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="268"/>
-      <c r="D34" s="227" t="s">
+      <c r="C34" s="285"/>
+      <c r="D34" s="356" t="s">
         <v>304</v>
       </c>
-      <c r="E34" s="237"/>
-      <c r="F34" s="242" t="s">
+      <c r="E34" s="238"/>
+      <c r="F34" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="237"/>
-      <c r="H34" s="284" t="s">
+      <c r="G34" s="238"/>
+      <c r="H34" s="363" t="s">
         <v>77</v>
       </c>
-      <c r="I34" s="285"/>
-      <c r="J34" s="229" t="s">
+      <c r="I34" s="406"/>
+      <c r="J34" s="336" t="s">
         <v>149</v>
       </c>
-      <c r="K34" s="320"/>
+      <c r="K34" s="338"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -7521,25 +7516,25 @@
       <c r="AB34" s="3"/>
     </row>
     <row r="35" spans="1:28" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="267"/>
+      <c r="A35" s="284"/>
       <c r="B35" s="50" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="288" t="s">
+      <c r="D35" s="361" t="s">
         <v>140</v>
       </c>
-      <c r="E35" s="289"/>
-      <c r="F35" s="242" t="s">
+      <c r="E35" s="362"/>
+      <c r="F35" s="237" t="s">
         <v>73</v>
       </c>
-      <c r="G35" s="237"/>
-      <c r="H35" s="227" t="s">
+      <c r="G35" s="238"/>
+      <c r="H35" s="356" t="s">
         <v>266</v>
       </c>
-      <c r="I35" s="237"/>
+      <c r="I35" s="238"/>
       <c r="J35" s="78"/>
       <c r="K35" s="97"/>
       <c r="L35" s="2"/>
@@ -7561,25 +7556,25 @@
       <c r="AB35" s="3"/>
     </row>
     <row r="36" spans="1:28" ht="53.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="268"/>
+      <c r="A36" s="285"/>
       <c r="B36" s="51" t="s">
         <v>24</v>
       </c>
       <c r="C36" s="174" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="294" t="s">
+      <c r="D36" s="315" t="s">
         <v>170</v>
       </c>
-      <c r="E36" s="295"/>
-      <c r="F36" s="270" t="s">
+      <c r="E36" s="369"/>
+      <c r="F36" s="393" t="s">
         <v>66</v>
       </c>
-      <c r="G36" s="271"/>
-      <c r="H36" s="296" t="s">
+      <c r="G36" s="394"/>
+      <c r="H36" s="370" t="s">
         <v>335</v>
       </c>
-      <c r="I36" s="297"/>
+      <c r="I36" s="371"/>
       <c r="J36" s="161" t="s">
         <v>201</v>
       </c>
@@ -7606,10 +7601,10 @@
     </row>
     <row r="37" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="52"/>
-      <c r="B37" s="415" t="s">
+      <c r="B37" s="230" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="244"/>
+      <c r="C37" s="231"/>
       <c r="D37" s="47"/>
       <c r="E37" s="48"/>
       <c r="F37" s="48"/>
@@ -7637,7 +7632,7 @@
       <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="1:28" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="350" t="s">
+      <c r="A38" s="322" t="s">
         <v>27</v>
       </c>
       <c r="B38" s="183" t="s">
@@ -7687,7 +7682,7 @@
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="351"/>
+      <c r="A39" s="323"/>
       <c r="B39" s="64" t="s">
         <v>221</v>
       </c>
@@ -7700,14 +7695,14 @@
       <c r="E39" s="194" t="s">
         <v>331</v>
       </c>
-      <c r="F39" s="393" t="s">
+      <c r="F39" s="258" t="s">
         <v>219</v>
       </c>
-      <c r="G39" s="394"/>
-      <c r="H39" s="394"/>
-      <c r="I39" s="394"/>
-      <c r="J39" s="394"/>
-      <c r="K39" s="395"/>
+      <c r="G39" s="259"/>
+      <c r="H39" s="259"/>
+      <c r="I39" s="259"/>
+      <c r="J39" s="259"/>
+      <c r="K39" s="260"/>
       <c r="L39" s="109"/>
       <c r="M39" s="109"/>
       <c r="N39" s="109"/>
@@ -7727,11 +7722,11 @@
       <c r="AB39" s="110"/>
     </row>
     <row r="40" spans="1:28" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="267"/>
+      <c r="A40" s="284"/>
       <c r="B40" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="416" t="s">
+      <c r="C40" s="232" t="s">
         <v>28</v>
       </c>
       <c r="D40" s="186" t="s">
@@ -7740,14 +7735,14 @@
       <c r="E40" s="163" t="s">
         <v>285</v>
       </c>
-      <c r="F40" s="243" t="s">
+      <c r="F40" s="241" t="s">
         <v>96</v>
       </c>
-      <c r="G40" s="421"/>
-      <c r="H40" s="242" t="s">
+      <c r="G40" s="242"/>
+      <c r="H40" s="237" t="s">
         <v>116</v>
       </c>
-      <c r="I40" s="237"/>
+      <c r="I40" s="238"/>
       <c r="J40" s="96"/>
       <c r="K40" s="100"/>
       <c r="L40" s="2"/>
@@ -7769,11 +7764,11 @@
       <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="267"/>
+      <c r="A41" s="284"/>
       <c r="B41" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="417"/>
+      <c r="C41" s="233"/>
       <c r="D41" s="187" t="s">
         <v>247</v>
       </c>
@@ -7786,10 +7781,10 @@
       <c r="G41" s="44" t="s">
         <v>255</v>
       </c>
-      <c r="H41" s="276" t="s">
+      <c r="H41" s="271" t="s">
         <v>319</v>
       </c>
-      <c r="I41" s="277"/>
+      <c r="I41" s="272"/>
       <c r="J41" s="164"/>
       <c r="K41" s="108"/>
       <c r="L41" s="2"/>
@@ -7811,15 +7806,15 @@
       <c r="AB41" s="3"/>
     </row>
     <row r="42" spans="1:28" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="267"/>
+      <c r="A42" s="284"/>
       <c r="B42" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="418"/>
-      <c r="D42" s="247" t="s">
+      <c r="C42" s="234"/>
+      <c r="D42" s="399" t="s">
         <v>269</v>
       </c>
-      <c r="E42" s="248"/>
+      <c r="E42" s="342"/>
       <c r="F42" s="165" t="s">
         <v>256</v>
       </c>
@@ -7830,12 +7825,12 @@
         <v>315</v>
       </c>
       <c r="I42" s="198" t="s">
-        <v>343</v>
-      </c>
-      <c r="J42" s="263" t="s">
+        <v>350</v>
+      </c>
+      <c r="J42" s="389" t="s">
         <v>173</v>
       </c>
-      <c r="K42" s="264"/>
+      <c r="K42" s="390"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -7855,31 +7850,31 @@
       <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="1:28" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="267"/>
+      <c r="A43" s="284"/>
       <c r="B43" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="419" t="s">
+      <c r="C43" s="235" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="238" t="s">
+      <c r="D43" s="224" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="356"/>
-      <c r="F43" s="253" t="s">
+      <c r="E43" s="254"/>
+      <c r="F43" s="221" t="s">
         <v>55</v>
       </c>
-      <c r="G43" s="253"/>
+      <c r="G43" s="221"/>
       <c r="H43" s="180" t="s">
         <v>180</v>
       </c>
       <c r="I43" s="169" t="s">
         <v>148</v>
       </c>
-      <c r="J43" s="217" t="s">
+      <c r="J43" s="265" t="s">
         <v>65</v>
       </c>
-      <c r="K43" s="235"/>
+      <c r="K43" s="420"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -7899,29 +7894,29 @@
       <c r="AB43" s="3"/>
     </row>
     <row r="44" spans="1:28" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="267"/>
+      <c r="A44" s="284"/>
       <c r="B44" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="417"/>
-      <c r="D44" s="356" t="s">
+      <c r="C44" s="233"/>
+      <c r="D44" s="254" t="s">
         <v>112</v>
       </c>
-      <c r="E44" s="239"/>
-      <c r="F44" s="217" t="s">
+      <c r="E44" s="225"/>
+      <c r="F44" s="265" t="s">
         <v>314</v>
       </c>
-      <c r="G44" s="218"/>
+      <c r="G44" s="266"/>
       <c r="H44" s="43" t="s">
         <v>115</v>
       </c>
       <c r="I44" s="123" t="s">
         <v>71</v>
       </c>
-      <c r="J44" s="302" t="s">
+      <c r="J44" s="375" t="s">
         <v>153</v>
       </c>
-      <c r="K44" s="303"/>
+      <c r="K44" s="376"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -7941,29 +7936,29 @@
       <c r="AB44" s="3"/>
     </row>
     <row r="45" spans="1:28" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="267"/>
+      <c r="A45" s="284"/>
       <c r="B45" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="417"/>
-      <c r="D45" s="238" t="s">
+      <c r="C45" s="233"/>
+      <c r="D45" s="224" t="s">
         <v>265</v>
       </c>
-      <c r="E45" s="356"/>
+      <c r="E45" s="254"/>
       <c r="F45" s="44" t="s">
         <v>236</v>
       </c>
-      <c r="G45" s="253" t="s">
+      <c r="G45" s="221" t="s">
         <v>292</v>
       </c>
-      <c r="H45" s="246"/>
+      <c r="H45" s="227"/>
       <c r="I45" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="J45" s="302" t="s">
+      <c r="J45" s="375" t="s">
         <v>167</v>
       </c>
-      <c r="K45" s="303"/>
+      <c r="K45" s="376"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -7983,26 +7978,26 @@
       <c r="AB45" s="3"/>
     </row>
     <row r="46" spans="1:28" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="267"/>
+      <c r="A46" s="284"/>
       <c r="B46" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="417"/>
-      <c r="D46" s="238" t="s">
+      <c r="C46" s="233"/>
+      <c r="D46" s="224" t="s">
         <v>277</v>
       </c>
-      <c r="E46" s="255"/>
+      <c r="E46" s="313"/>
       <c r="F46" s="44" t="s">
         <v>320</v>
       </c>
-      <c r="G46" s="242" t="s">
+      <c r="G46" s="237" t="s">
         <v>67</v>
       </c>
-      <c r="H46" s="237"/>
-      <c r="I46" s="298" t="s">
+      <c r="H46" s="238"/>
+      <c r="I46" s="372" t="s">
         <v>307</v>
       </c>
-      <c r="J46" s="299"/>
+      <c r="J46" s="243"/>
       <c r="K46" s="97"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
@@ -8023,13 +8018,13 @@
       <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28" ht="64.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="267"/>
+      <c r="A47" s="284"/>
       <c r="B47" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="417"/>
-      <c r="D47" s="299"/>
-      <c r="E47" s="340"/>
+      <c r="C47" s="233"/>
+      <c r="D47" s="243"/>
+      <c r="E47" s="244"/>
       <c r="F47" s="53"/>
       <c r="G47" s="42"/>
       <c r="H47" s="107"/>
@@ -8055,11 +8050,11 @@
       <c r="AB47" s="3"/>
     </row>
     <row r="48" spans="1:28" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="267"/>
+      <c r="A48" s="284"/>
       <c r="B48" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="417"/>
+      <c r="C48" s="233"/>
       <c r="D48" s="188" t="s">
         <v>120</v>
       </c>
@@ -8072,14 +8067,14 @@
       <c r="G48" s="172" t="s">
         <v>104</v>
       </c>
-      <c r="H48" s="253" t="s">
+      <c r="H48" s="221" t="s">
         <v>215</v>
       </c>
-      <c r="I48" s="246"/>
-      <c r="J48" s="304" t="s">
+      <c r="I48" s="227"/>
+      <c r="J48" s="377" t="s">
         <v>211</v>
       </c>
-      <c r="K48" s="305"/>
+      <c r="K48" s="378"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -8099,23 +8094,23 @@
       <c r="AB48" s="3"/>
     </row>
     <row r="49" spans="1:28" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="267"/>
+      <c r="A49" s="284"/>
       <c r="B49" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="417"/>
-      <c r="D49" s="293" t="s">
+      <c r="C49" s="233"/>
+      <c r="D49" s="367" t="s">
         <v>195</v>
       </c>
-      <c r="E49" s="256"/>
-      <c r="F49" s="306" t="s">
+      <c r="E49" s="368"/>
+      <c r="F49" s="239" t="s">
         <v>219</v>
       </c>
-      <c r="G49" s="307"/>
-      <c r="H49" s="306" t="s">
+      <c r="G49" s="240"/>
+      <c r="H49" s="239" t="s">
         <v>210</v>
       </c>
-      <c r="I49" s="307"/>
+      <c r="I49" s="240"/>
       <c r="J49" s="166" t="s">
         <v>57</v>
       </c>
@@ -8141,27 +8136,27 @@
       <c r="AB49" s="3"/>
     </row>
     <row r="50" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="267"/>
+      <c r="A50" s="284"/>
       <c r="B50" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="417"/>
-      <c r="D50" s="218" t="s">
+      <c r="C50" s="233"/>
+      <c r="D50" s="266" t="s">
         <v>339</v>
       </c>
-      <c r="E50" s="246"/>
-      <c r="F50" s="253" t="s">
+      <c r="E50" s="227"/>
+      <c r="F50" s="221" t="s">
         <v>340</v>
       </c>
-      <c r="G50" s="246"/>
-      <c r="H50" s="253" t="s">
+      <c r="G50" s="227"/>
+      <c r="H50" s="221" t="s">
         <v>192</v>
       </c>
-      <c r="I50" s="246"/>
-      <c r="J50" s="300" t="s">
+      <c r="I50" s="227"/>
+      <c r="J50" s="373" t="s">
         <v>190</v>
       </c>
-      <c r="K50" s="301"/>
+      <c r="K50" s="374"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -8181,23 +8176,23 @@
       <c r="AB50" s="3"/>
     </row>
     <row r="51" spans="1:28" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="267"/>
+      <c r="A51" s="284"/>
       <c r="B51" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="418"/>
-      <c r="D51" s="218" t="s">
+      <c r="C51" s="234"/>
+      <c r="D51" s="266" t="s">
         <v>286</v>
       </c>
-      <c r="E51" s="246"/>
-      <c r="F51" s="253" t="s">
+      <c r="E51" s="227"/>
+      <c r="F51" s="221" t="s">
         <v>191</v>
       </c>
-      <c r="G51" s="246"/>
-      <c r="H51" s="253" t="s">
+      <c r="G51" s="227"/>
+      <c r="H51" s="221" t="s">
         <v>287</v>
       </c>
-      <c r="I51" s="246"/>
+      <c r="I51" s="227"/>
       <c r="J51" s="77"/>
       <c r="K51" s="97"/>
       <c r="L51" s="2"/>
@@ -8219,25 +8214,25 @@
       <c r="AB51" s="3"/>
     </row>
     <row r="52" spans="1:28" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="267"/>
+      <c r="A52" s="284"/>
       <c r="B52" s="184" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="190" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="253" t="s">
+      <c r="D52" s="221" t="s">
         <v>216</v>
       </c>
-      <c r="E52" s="246"/>
-      <c r="F52" s="253" t="s">
+      <c r="E52" s="227"/>
+      <c r="F52" s="221" t="s">
         <v>156</v>
       </c>
-      <c r="G52" s="246"/>
-      <c r="H52" s="253" t="s">
+      <c r="G52" s="227"/>
+      <c r="H52" s="221" t="s">
         <v>142</v>
       </c>
-      <c r="I52" s="246"/>
+      <c r="I52" s="227"/>
       <c r="J52" s="76"/>
       <c r="K52" s="97"/>
       <c r="L52" s="2"/>
@@ -8259,7 +8254,7 @@
       <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="1:28" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="268"/>
+      <c r="A53" s="285"/>
       <c r="B53" s="185" t="s">
         <v>24</v>
       </c>
@@ -8272,14 +8267,14 @@
       <c r="E53" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="F53" s="354" t="s">
+      <c r="F53" s="326" t="s">
         <v>158</v>
       </c>
-      <c r="G53" s="355"/>
-      <c r="H53" s="406" t="s">
+      <c r="G53" s="327"/>
+      <c r="H53" s="278" t="s">
         <v>109</v>
       </c>
-      <c r="I53" s="345"/>
+      <c r="I53" s="279"/>
       <c r="J53" s="73" t="s">
         <v>110</v>
       </c>
@@ -8304,10 +8299,10 @@
     </row>
     <row r="54" spans="1:28" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="57"/>
-      <c r="B54" s="420" t="s">
+      <c r="B54" s="236" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="410"/>
+      <c r="C54" s="218"/>
       <c r="D54" s="47"/>
       <c r="E54" s="58"/>
       <c r="F54" s="58"/>
@@ -8335,7 +8330,7 @@
       <c r="AB54" s="3"/>
     </row>
     <row r="55" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="368" t="s">
+      <c r="A55" s="309" t="s">
         <v>31</v>
       </c>
       <c r="B55" s="116" t="s">
@@ -8385,25 +8380,25 @@
       <c r="AB55" s="3"/>
     </row>
     <row r="56" spans="1:28" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="369"/>
+      <c r="A56" s="310"/>
       <c r="B56" s="64" t="s">
         <v>220</v>
       </c>
       <c r="C56" s="114"/>
       <c r="D56" s="201" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E56" s="201" t="s">
-        <v>348</v>
-      </c>
-      <c r="F56" s="396" t="s">
+        <v>346</v>
+      </c>
+      <c r="F56" s="261" t="s">
         <v>219</v>
       </c>
-      <c r="G56" s="396"/>
-      <c r="H56" s="396"/>
-      <c r="I56" s="396"/>
-      <c r="J56" s="397"/>
-      <c r="K56" s="398"/>
+      <c r="G56" s="261"/>
+      <c r="H56" s="261"/>
+      <c r="I56" s="261"/>
+      <c r="J56" s="262"/>
+      <c r="K56" s="263"/>
       <c r="L56" s="109"/>
       <c r="M56" s="109"/>
       <c r="N56" s="109"/>
@@ -8423,31 +8418,31 @@
       <c r="AB56" s="110"/>
     </row>
     <row r="57" spans="1:28" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="370"/>
+      <c r="A57" s="311"/>
       <c r="B57" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="357" t="s">
+      <c r="C57" s="330" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="352" t="s">
+      <c r="D57" s="324" t="s">
         <v>118</v>
       </c>
-      <c r="E57" s="360"/>
+      <c r="E57" s="333"/>
       <c r="F57" s="44" t="s">
         <v>328</v>
       </c>
       <c r="G57" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="H57" s="356" t="s">
+      <c r="H57" s="254" t="s">
         <v>143</v>
       </c>
-      <c r="I57" s="239"/>
-      <c r="J57" s="261" t="s">
+      <c r="I57" s="225"/>
+      <c r="J57" s="269" t="s">
         <v>204</v>
       </c>
-      <c r="K57" s="262"/>
+      <c r="K57" s="270"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -8467,29 +8462,29 @@
       <c r="AB57" s="3"/>
     </row>
     <row r="58" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="370"/>
+      <c r="A58" s="311"/>
       <c r="B58" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="246"/>
-      <c r="D58" s="253" t="s">
+      <c r="C58" s="227"/>
+      <c r="D58" s="221" t="s">
         <v>325</v>
       </c>
-      <c r="E58" s="246"/>
+      <c r="E58" s="227"/>
       <c r="F58" s="44" t="s">
         <v>232</v>
       </c>
       <c r="G58" s="44" t="s">
         <v>283</v>
       </c>
-      <c r="H58" s="317" t="s">
+      <c r="H58" s="267" t="s">
         <v>168</v>
       </c>
-      <c r="I58" s="246"/>
-      <c r="J58" s="352" t="s">
+      <c r="I58" s="227"/>
+      <c r="J58" s="324" t="s">
         <v>146</v>
       </c>
-      <c r="K58" s="353"/>
+      <c r="K58" s="325"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -8509,11 +8504,11 @@
       <c r="AB58" s="3"/>
     </row>
     <row r="59" spans="1:28" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="370"/>
+      <c r="A59" s="311"/>
       <c r="B59" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="246"/>
+      <c r="C59" s="227"/>
       <c r="D59" s="44" t="s">
         <v>234</v>
       </c>
@@ -8529,10 +8524,10 @@
       <c r="H59" s="44" t="s">
         <v>323</v>
       </c>
-      <c r="I59" s="317" t="s">
+      <c r="I59" s="267" t="s">
         <v>111</v>
       </c>
-      <c r="J59" s="274"/>
+      <c r="J59" s="317"/>
       <c r="K59" s="97"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
@@ -8553,11 +8548,11 @@
       <c r="AB59" s="3"/>
     </row>
     <row r="60" spans="1:28" ht="63" x14ac:dyDescent="0.25">
-      <c r="A60" s="370"/>
+      <c r="A60" s="311"/>
       <c r="B60" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="358" t="s">
+      <c r="C60" s="331" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="44" t="s">
@@ -8578,10 +8573,10 @@
       <c r="I60" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="J60" s="253" t="s">
+      <c r="J60" s="221" t="s">
         <v>213</v>
       </c>
-      <c r="K60" s="378"/>
+      <c r="K60" s="318"/>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -8601,26 +8596,26 @@
       <c r="AB60" s="3"/>
     </row>
     <row r="61" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="370"/>
+      <c r="A61" s="311"/>
       <c r="B61" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="246"/>
+      <c r="C61" s="227"/>
       <c r="D61" s="54"/>
       <c r="E61" s="202" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F61" s="198" t="s">
-        <v>347</v>
-      </c>
-      <c r="H61" s="253" t="s">
+        <v>345</v>
+      </c>
+      <c r="H61" s="221" t="s">
         <v>284</v>
       </c>
-      <c r="I61" s="246"/>
-      <c r="J61" s="400" t="s">
+      <c r="I61" s="227"/>
+      <c r="J61" s="252" t="s">
         <v>159</v>
       </c>
-      <c r="K61" s="401"/>
+      <c r="K61" s="253"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8640,11 +8635,11 @@
       <c r="AB61" s="3"/>
     </row>
     <row r="62" spans="1:28" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="370"/>
+      <c r="A62" s="311"/>
       <c r="B62" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="246"/>
+      <c r="C62" s="227"/>
       <c r="D62" s="198" t="s">
         <v>157</v>
       </c>
@@ -8663,10 +8658,10 @@
       <c r="I62" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="J62" s="400" t="s">
+      <c r="J62" s="252" t="s">
         <v>205</v>
       </c>
-      <c r="K62" s="401"/>
+      <c r="K62" s="253"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8686,19 +8681,19 @@
       <c r="AB62" s="3"/>
     </row>
     <row r="63" spans="1:28" ht="63" x14ac:dyDescent="0.25">
-      <c r="A63" s="370"/>
+      <c r="A63" s="311"/>
       <c r="B63" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="246"/>
-      <c r="D63" s="317" t="s">
+      <c r="C63" s="227"/>
+      <c r="D63" s="267" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="246"/>
-      <c r="F63" s="253" t="s">
+      <c r="E63" s="227"/>
+      <c r="F63" s="221" t="s">
         <v>279</v>
       </c>
-      <c r="G63" s="246"/>
+      <c r="G63" s="227"/>
       <c r="H63" s="44" t="s">
         <v>290</v>
       </c>
@@ -8730,11 +8725,11 @@
       <c r="AB63" s="3"/>
     </row>
     <row r="64" spans="1:28" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="370"/>
+      <c r="A64" s="311"/>
       <c r="B64" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="246"/>
+      <c r="C64" s="227"/>
       <c r="D64" s="44" t="s">
         <v>282</v>
       </c>
@@ -8747,14 +8742,14 @@
       <c r="G64" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="H64" s="408" t="s">
+      <c r="H64" s="281" t="s">
         <v>268</v>
       </c>
-      <c r="I64" s="249"/>
-      <c r="J64" s="317" t="s">
+      <c r="I64" s="282"/>
+      <c r="J64" s="267" t="s">
         <v>164</v>
       </c>
-      <c r="K64" s="399"/>
+      <c r="K64" s="268"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8774,27 +8769,27 @@
       <c r="AB64" s="3"/>
     </row>
     <row r="65" spans="1:28" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="370"/>
+      <c r="A65" s="311"/>
       <c r="B65" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="246"/>
-      <c r="D65" s="253" t="s">
+      <c r="C65" s="227"/>
+      <c r="D65" s="221" t="s">
         <v>318</v>
       </c>
-      <c r="E65" s="246"/>
-      <c r="F65" s="313" t="s">
+      <c r="E65" s="227"/>
+      <c r="F65" s="328" t="s">
         <v>219</v>
       </c>
-      <c r="G65" s="314"/>
-      <c r="H65" s="313" t="s">
+      <c r="G65" s="329"/>
+      <c r="H65" s="328" t="s">
         <v>219</v>
       </c>
-      <c r="I65" s="314"/>
-      <c r="J65" s="317" t="s">
+      <c r="I65" s="329"/>
+      <c r="J65" s="267" t="s">
         <v>196</v>
       </c>
-      <c r="K65" s="399"/>
+      <c r="K65" s="268"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8814,29 +8809,29 @@
       <c r="AB65" s="3"/>
     </row>
     <row r="66" spans="1:28" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="370"/>
+      <c r="A66" s="311"/>
       <c r="B66" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="C66" s="359" t="s">
+      <c r="C66" s="332" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="317" t="s">
+      <c r="D66" s="267" t="s">
         <v>193</v>
       </c>
-      <c r="E66" s="246"/>
-      <c r="F66" s="317" t="s">
+      <c r="E66" s="227"/>
+      <c r="F66" s="267" t="s">
         <v>194</v>
       </c>
-      <c r="G66" s="246"/>
-      <c r="H66" s="317" t="s">
+      <c r="G66" s="227"/>
+      <c r="H66" s="267" t="s">
         <v>134</v>
       </c>
-      <c r="I66" s="246"/>
-      <c r="J66" s="400" t="s">
+      <c r="I66" s="227"/>
+      <c r="J66" s="252" t="s">
         <v>206</v>
       </c>
-      <c r="K66" s="401"/>
+      <c r="K66" s="253"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -8856,27 +8851,27 @@
       <c r="AB66" s="3"/>
     </row>
     <row r="67" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="370"/>
+      <c r="A67" s="311"/>
       <c r="B67" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="C67" s="246"/>
-      <c r="D67" s="253" t="s">
+      <c r="C67" s="227"/>
+      <c r="D67" s="221" t="s">
         <v>288</v>
       </c>
-      <c r="E67" s="246"/>
-      <c r="F67" s="253" t="s">
+      <c r="E67" s="227"/>
+      <c r="F67" s="221" t="s">
         <v>289</v>
       </c>
-      <c r="G67" s="246"/>
-      <c r="H67" s="317" t="s">
+      <c r="G67" s="227"/>
+      <c r="H67" s="267" t="s">
         <v>119</v>
       </c>
-      <c r="I67" s="246"/>
-      <c r="J67" s="413" t="s">
+      <c r="I67" s="227"/>
+      <c r="J67" s="228" t="s">
         <v>145</v>
       </c>
-      <c r="K67" s="414"/>
+      <c r="K67" s="229"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8896,25 +8891,25 @@
       <c r="AB67" s="3"/>
     </row>
     <row r="68" spans="1:28" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="370"/>
+      <c r="A68" s="311"/>
       <c r="B68" s="118" t="s">
         <v>23</v>
       </c>
       <c r="C68" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="D68" s="253" t="s">
+      <c r="D68" s="221" t="s">
         <v>341</v>
       </c>
-      <c r="E68" s="246"/>
-      <c r="F68" s="253" t="s">
+      <c r="E68" s="227"/>
+      <c r="F68" s="221" t="s">
         <v>113</v>
       </c>
-      <c r="G68" s="246"/>
-      <c r="H68" s="253" t="s">
+      <c r="G68" s="227"/>
+      <c r="H68" s="221" t="s">
         <v>217</v>
       </c>
-      <c r="I68" s="246"/>
+      <c r="I68" s="227"/>
       <c r="J68" s="79"/>
       <c r="K68" s="97"/>
       <c r="L68" s="2"/>
@@ -8936,7 +8931,7 @@
       <c r="AB68" s="3"/>
     </row>
     <row r="69" spans="1:28" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="371"/>
+      <c r="A69" s="312"/>
       <c r="B69" s="119" t="s">
         <v>24</v>
       </c>
@@ -8959,7 +8954,7 @@
         <v>315</v>
       </c>
       <c r="I69" s="197" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="J69" s="168" t="s">
         <v>69</v>
@@ -8985,10 +8980,10 @@
     </row>
     <row r="70" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="125"/>
-      <c r="B70" s="379" t="s">
+      <c r="B70" s="319" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="380"/>
+      <c r="C70" s="320"/>
       <c r="D70" s="126"/>
       <c r="E70" s="127"/>
       <c r="F70" s="127"/>
@@ -9016,7 +9011,7 @@
       <c r="AB70" s="3"/>
     </row>
     <row r="71" spans="1:28" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="361" t="s">
+      <c r="A71" s="299" t="s">
         <v>34</v>
       </c>
       <c r="B71" s="30" t="s">
@@ -9035,7 +9030,7 @@
       <c r="G71" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="H71" s="402" t="s">
+      <c r="H71" s="274" t="s">
         <v>123</v>
       </c>
       <c r="I71" s="136" t="s">
@@ -9045,7 +9040,7 @@
         <v>40</v>
       </c>
       <c r="K71" s="106" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -9066,24 +9061,24 @@
       <c r="AB71" s="3"/>
     </row>
     <row r="72" spans="1:28" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="362"/>
+      <c r="A72" s="300"/>
       <c r="B72" s="179" t="s">
         <v>313</v>
       </c>
-      <c r="C72" s="388" t="s">
+      <c r="C72" s="297" t="s">
         <v>227</v>
       </c>
       <c r="D72" s="176"/>
       <c r="E72" s="177"/>
-      <c r="F72" s="377" t="s">
+      <c r="F72" s="223" t="s">
         <v>224</v>
       </c>
-      <c r="G72" s="261"/>
-      <c r="H72" s="403"/>
-      <c r="I72" s="377" t="s">
+      <c r="G72" s="269"/>
+      <c r="H72" s="275"/>
+      <c r="I72" s="223" t="s">
         <v>317</v>
       </c>
-      <c r="J72" s="377"/>
+      <c r="J72" s="223"/>
       <c r="K72" s="175"/>
       <c r="L72" s="109"/>
       <c r="M72" s="109"/>
@@ -9104,25 +9099,25 @@
       <c r="AB72" s="110"/>
     </row>
     <row r="73" spans="1:28" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="363"/>
+      <c r="A73" s="301"/>
       <c r="B73" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="C73" s="389"/>
-      <c r="D73" s="425" t="s">
+      <c r="C73" s="298"/>
+      <c r="D73" s="250" t="s">
         <v>218</v>
       </c>
-      <c r="E73" s="426"/>
-      <c r="F73" s="372" t="s">
+      <c r="E73" s="251"/>
+      <c r="F73" s="245" t="s">
         <v>219</v>
       </c>
-      <c r="G73" s="373"/>
-      <c r="H73" s="404"/>
-      <c r="I73" s="422" t="s">
+      <c r="G73" s="246"/>
+      <c r="H73" s="276"/>
+      <c r="I73" s="247" t="s">
         <v>219</v>
       </c>
-      <c r="J73" s="423"/>
-      <c r="K73" s="424"/>
+      <c r="J73" s="248"/>
+      <c r="K73" s="249"/>
       <c r="L73" s="109"/>
       <c r="M73" s="109"/>
       <c r="N73" s="109"/>
@@ -9142,26 +9137,26 @@
       <c r="AB73" s="110"/>
     </row>
     <row r="74" spans="1:28" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="364"/>
+      <c r="A74" s="302"/>
       <c r="B74" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="381" t="s">
+      <c r="C74" s="283" t="s">
         <v>41</v>
       </c>
-      <c r="D74" s="376" t="s">
+      <c r="D74" s="222" t="s">
         <v>276</v>
       </c>
-      <c r="E74" s="377"/>
-      <c r="F74" s="383" t="s">
-        <v>350</v>
-      </c>
-      <c r="G74" s="349"/>
-      <c r="H74" s="404"/>
-      <c r="I74" s="376" t="s">
+      <c r="E74" s="223"/>
+      <c r="F74" s="289" t="s">
+        <v>348</v>
+      </c>
+      <c r="G74" s="290"/>
+      <c r="H74" s="276"/>
+      <c r="I74" s="222" t="s">
         <v>336</v>
       </c>
-      <c r="J74" s="377"/>
+      <c r="J74" s="223"/>
       <c r="K74" s="124"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
@@ -9182,24 +9177,24 @@
       <c r="AB74" s="3"/>
     </row>
     <row r="75" spans="1:28" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="364"/>
+      <c r="A75" s="302"/>
       <c r="B75" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="267"/>
-      <c r="D75" s="376" t="s">
+      <c r="C75" s="284"/>
+      <c r="D75" s="222" t="s">
         <v>298</v>
       </c>
-      <c r="E75" s="377"/>
-      <c r="F75" s="253" t="s">
+      <c r="E75" s="223"/>
+      <c r="F75" s="221" t="s">
         <v>326</v>
       </c>
-      <c r="G75" s="387"/>
-      <c r="H75" s="404"/>
-      <c r="I75" s="231" t="s">
+      <c r="G75" s="295"/>
+      <c r="H75" s="276"/>
+      <c r="I75" s="316" t="s">
         <v>160</v>
       </c>
-      <c r="J75" s="231"/>
+      <c r="J75" s="316"/>
       <c r="K75" s="97"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
@@ -9220,26 +9215,26 @@
       <c r="AB75" s="3"/>
     </row>
     <row r="76" spans="1:28" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="364"/>
+      <c r="A76" s="302"/>
       <c r="B76" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C76" s="268"/>
-      <c r="D76" s="236" t="s">
+      <c r="C76" s="285"/>
+      <c r="D76" s="287" t="s">
         <v>135</v>
       </c>
-      <c r="E76" s="382"/>
+      <c r="E76" s="288"/>
       <c r="F76" s="71" t="s">
         <v>233</v>
       </c>
       <c r="G76" s="150" t="s">
         <v>282</v>
       </c>
-      <c r="H76" s="404"/>
-      <c r="I76" s="375" t="s">
+      <c r="H76" s="276"/>
+      <c r="I76" s="273" t="s">
         <v>209</v>
       </c>
-      <c r="J76" s="239"/>
+      <c r="J76" s="225"/>
       <c r="K76" s="97"/>
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
@@ -9260,26 +9255,26 @@
       <c r="AB76" s="3"/>
     </row>
     <row r="77" spans="1:28" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="364"/>
+      <c r="A77" s="302"/>
       <c r="B77" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C77" s="269" t="s">
+      <c r="C77" s="286" t="s">
         <v>15</v>
       </c>
-      <c r="D77" s="384" t="s">
+      <c r="D77" s="291" t="s">
         <v>333</v>
       </c>
-      <c r="E77" s="385"/>
-      <c r="F77" s="217" t="s">
+      <c r="E77" s="292"/>
+      <c r="F77" s="265" t="s">
         <v>222</v>
       </c>
-      <c r="G77" s="218"/>
-      <c r="H77" s="404"/>
-      <c r="I77" s="375" t="s">
+      <c r="G77" s="266"/>
+      <c r="H77" s="276"/>
+      <c r="I77" s="273" t="s">
         <v>62</v>
       </c>
-      <c r="J77" s="239"/>
+      <c r="J77" s="225"/>
       <c r="K77" s="97"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
@@ -9300,26 +9295,26 @@
       <c r="AB77" s="3"/>
     </row>
     <row r="78" spans="1:28" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="364"/>
+      <c r="A78" s="302"/>
       <c r="B78" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C78" s="267"/>
+      <c r="C78" s="284"/>
       <c r="D78" s="65" t="s">
         <v>105</v>
       </c>
       <c r="E78" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="F78" s="386" t="s">
+      <c r="F78" s="293" t="s">
         <v>225</v>
       </c>
-      <c r="G78" s="330"/>
-      <c r="H78" s="404"/>
-      <c r="I78" s="375" t="s">
+      <c r="G78" s="294"/>
+      <c r="H78" s="276"/>
+      <c r="I78" s="273" t="s">
         <v>182</v>
       </c>
-      <c r="J78" s="239"/>
+      <c r="J78" s="225"/>
       <c r="K78" s="97"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
@@ -9340,28 +9335,28 @@
       <c r="AB78" s="3"/>
     </row>
     <row r="79" spans="1:28" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="364"/>
+      <c r="A79" s="302"/>
       <c r="B79" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C79" s="267"/>
-      <c r="D79" s="238" t="s">
+      <c r="C79" s="284"/>
+      <c r="D79" s="224" t="s">
         <v>231</v>
       </c>
-      <c r="E79" s="330"/>
+      <c r="E79" s="294"/>
       <c r="F79" s="170" t="s">
         <v>258</v>
       </c>
       <c r="G79" s="171" t="s">
         <v>259</v>
       </c>
-      <c r="H79" s="404"/>
-      <c r="I79" s="375" t="s">
+      <c r="H79" s="276"/>
+      <c r="I79" s="273" t="s">
         <v>181</v>
       </c>
-      <c r="J79" s="239"/>
+      <c r="J79" s="225"/>
       <c r="K79" s="200" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
@@ -9382,11 +9377,11 @@
       <c r="AB79" s="3"/>
     </row>
     <row r="80" spans="1:28" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="364"/>
+      <c r="A80" s="302"/>
       <c r="B80" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="267"/>
+      <c r="C80" s="284"/>
       <c r="D80" s="151" t="s">
         <v>238</v>
       </c>
@@ -9399,11 +9394,11 @@
       <c r="G80" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="H80" s="404"/>
-      <c r="I80" s="356" t="s">
+      <c r="H80" s="276"/>
+      <c r="I80" s="254" t="s">
         <v>83</v>
       </c>
-      <c r="J80" s="239"/>
+      <c r="J80" s="225"/>
       <c r="K80" s="97"/>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
@@ -9424,24 +9419,24 @@
       <c r="AB80" s="3"/>
     </row>
     <row r="81" spans="1:28" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="364"/>
+      <c r="A81" s="302"/>
       <c r="B81" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C81" s="267"/>
-      <c r="D81" s="356" t="s">
+      <c r="C81" s="284"/>
+      <c r="D81" s="254" t="s">
         <v>131</v>
       </c>
-      <c r="E81" s="374"/>
-      <c r="F81" s="319" t="s">
+      <c r="E81" s="314"/>
+      <c r="F81" s="264" t="s">
         <v>223</v>
       </c>
-      <c r="G81" s="239"/>
-      <c r="H81" s="404"/>
-      <c r="I81" s="356" t="s">
+      <c r="G81" s="225"/>
+      <c r="H81" s="276"/>
+      <c r="I81" s="254" t="s">
         <v>99</v>
       </c>
-      <c r="J81" s="239"/>
+      <c r="J81" s="225"/>
       <c r="K81" s="97"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
@@ -9462,24 +9457,24 @@
       <c r="AB81" s="3"/>
     </row>
     <row r="82" spans="1:28" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="364"/>
+      <c r="A82" s="302"/>
       <c r="B82" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="267"/>
-      <c r="D82" s="238" t="s">
+      <c r="C82" s="284"/>
+      <c r="D82" s="224" t="s">
         <v>162</v>
       </c>
-      <c r="E82" s="255"/>
-      <c r="F82" s="372" t="s">
+      <c r="E82" s="313"/>
+      <c r="F82" s="245" t="s">
         <v>219</v>
       </c>
-      <c r="G82" s="373"/>
-      <c r="H82" s="404"/>
-      <c r="I82" s="372" t="s">
+      <c r="G82" s="246"/>
+      <c r="H82" s="276"/>
+      <c r="I82" s="245" t="s">
         <v>161</v>
       </c>
-      <c r="J82" s="373"/>
+      <c r="J82" s="246"/>
       <c r="K82" s="98"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
@@ -9500,24 +9495,24 @@
       <c r="AB82" s="3"/>
     </row>
     <row r="83" spans="1:28" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="364"/>
+      <c r="A83" s="302"/>
       <c r="B83" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C83" s="267"/>
-      <c r="D83" s="238" t="s">
+      <c r="C83" s="284"/>
+      <c r="D83" s="224" t="s">
         <v>63</v>
       </c>
-      <c r="E83" s="340"/>
-      <c r="F83" s="319" t="s">
+      <c r="E83" s="244"/>
+      <c r="F83" s="264" t="s">
         <v>141</v>
       </c>
-      <c r="G83" s="239"/>
-      <c r="H83" s="404"/>
-      <c r="I83" s="238" t="s">
+      <c r="G83" s="225"/>
+      <c r="H83" s="276"/>
+      <c r="I83" s="224" t="s">
         <v>246</v>
       </c>
-      <c r="J83" s="239"/>
+      <c r="J83" s="225"/>
       <c r="K83" s="97"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
@@ -9538,16 +9533,16 @@
       <c r="AB83" s="3"/>
     </row>
     <row r="84" spans="1:28" ht="64.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="364"/>
+      <c r="A84" s="302"/>
       <c r="B84" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C84" s="267"/>
+      <c r="C84" s="284"/>
       <c r="D84" s="40"/>
       <c r="E84" s="41"/>
       <c r="F84" s="41"/>
       <c r="G84" s="67"/>
-      <c r="H84" s="404"/>
+      <c r="H84" s="276"/>
       <c r="I84" s="68"/>
       <c r="J84" s="80"/>
       <c r="K84" s="97"/>
@@ -9570,24 +9565,24 @@
       <c r="AB84" s="3"/>
     </row>
     <row r="85" spans="1:28" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="364"/>
+      <c r="A85" s="302"/>
       <c r="B85" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C85" s="268"/>
-      <c r="D85" s="238" t="s">
+      <c r="C85" s="285"/>
+      <c r="D85" s="224" t="s">
         <v>74</v>
       </c>
-      <c r="E85" s="340"/>
-      <c r="F85" s="286" t="s">
+      <c r="E85" s="244"/>
+      <c r="F85" s="296" t="s">
         <v>93</v>
       </c>
-      <c r="G85" s="239"/>
-      <c r="H85" s="404"/>
-      <c r="I85" s="238" t="s">
+      <c r="G85" s="225"/>
+      <c r="H85" s="276"/>
+      <c r="I85" s="224" t="s">
         <v>208</v>
       </c>
-      <c r="J85" s="239"/>
+      <c r="J85" s="225"/>
       <c r="K85" s="97"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
@@ -9608,26 +9603,26 @@
       <c r="AB85" s="3"/>
     </row>
     <row r="86" spans="1:28" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="364"/>
+      <c r="A86" s="302"/>
       <c r="B86" s="50" t="s">
         <v>23</v>
       </c>
       <c r="C86" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="D86" s="366" t="s">
+      <c r="D86" s="304" t="s">
         <v>186</v>
       </c>
-      <c r="E86" s="327"/>
-      <c r="F86" s="286" t="s">
+      <c r="E86" s="305"/>
+      <c r="F86" s="296" t="s">
         <v>185</v>
       </c>
-      <c r="G86" s="239"/>
-      <c r="H86" s="404"/>
-      <c r="I86" s="412" t="s">
+      <c r="G86" s="225"/>
+      <c r="H86" s="276"/>
+      <c r="I86" s="226" t="s">
         <v>207</v>
       </c>
-      <c r="J86" s="239"/>
+      <c r="J86" s="225"/>
       <c r="K86" s="97"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
@@ -9648,26 +9643,26 @@
       <c r="AB86" s="3"/>
     </row>
     <row r="87" spans="1:28" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="365"/>
+      <c r="A87" s="303"/>
       <c r="B87" s="51" t="s">
         <v>24</v>
       </c>
       <c r="C87" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D87" s="343" t="s">
+      <c r="D87" s="306" t="s">
         <v>79</v>
       </c>
-      <c r="E87" s="342"/>
-      <c r="F87" s="343" t="s">
+      <c r="E87" s="307"/>
+      <c r="F87" s="306" t="s">
         <v>80</v>
       </c>
-      <c r="G87" s="367"/>
-      <c r="H87" s="405"/>
-      <c r="I87" s="294" t="s">
+      <c r="G87" s="308"/>
+      <c r="H87" s="277"/>
+      <c r="I87" s="315" t="s">
         <v>78</v>
       </c>
-      <c r="J87" s="367"/>
+      <c r="J87" s="308"/>
       <c r="K87" s="99"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
@@ -37199,6 +37194,187 @@
     </row>
   </sheetData>
   <mergeCells count="205">
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="A22:A36"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="G1:J2"/>
+    <mergeCell ref="A2:E4"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C11:C20"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A38:A53"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="A71:A87"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="A55:A69"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="I80:J80"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C77:C85"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F39:K39"/>
+    <mergeCell ref="F56:K56"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="I79:J79"/>
+    <mergeCell ref="H71:H87"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J44:K44"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="F28:G28"/>
@@ -37223,187 +37399,6 @@
     <mergeCell ref="I81:J81"/>
     <mergeCell ref="I82:J82"/>
     <mergeCell ref="F63:G63"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F39:K39"/>
-    <mergeCell ref="F56:K56"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="I79:J79"/>
-    <mergeCell ref="H71:H87"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="C77:C85"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="A71:A87"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="A55:A69"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="I80:J80"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I87:J87"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="A38:A53"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="C60:C65"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="G1:J2"/>
-    <mergeCell ref="A2:E4"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C11:C20"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="A22:A36"/>
-    <mergeCell ref="C27:C34"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <pageMargins left="0.216187305364964" right="0.14099172089019399" top="0.26" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="25" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -37416,7 +37411,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>